<commit_message>
V2 started, using different crystal, ICM20948, 10 pin SWD header, and multiple component swaps
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Robots\STM32Quadcopter\STM32_SMD_Quadcopter_PCB_V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56837F8-0B21-4580-9969-319B9AFC7E46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C85645-A0AD-4F67-B265-988BA964D80E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Mounting holes, 4 corners</t>
   </si>
@@ -103,6 +103,54 @@
   </si>
   <si>
     <t>gps connector</t>
+  </si>
+  <si>
+    <t>all bottom components easy to solder, simple</t>
+  </si>
+  <si>
+    <t>as many as possible are simple</t>
+  </si>
+  <si>
+    <t>using ICM20948 because MPU6050 has no SPI bus</t>
+  </si>
+  <si>
+    <t>level shifter IC in use is merely N-channel MOSFET with sufficiently low Gate threshold voltage</t>
+  </si>
+  <si>
+    <t>switched crystal to 16MHz oscillator referenced in video</t>
+  </si>
+  <si>
+    <t>ICM20948</t>
+  </si>
+  <si>
+    <t>parts not in database at all:</t>
+  </si>
+  <si>
+    <t>tactile reset switch (unless we use an extended part)</t>
+  </si>
+  <si>
+    <t>parts not basic:</t>
+  </si>
+  <si>
+    <t>STM32F446RET6</t>
+  </si>
+  <si>
+    <t>SD card connector</t>
+  </si>
+  <si>
+    <t>USB connector</t>
+  </si>
+  <si>
+    <t>FT230XQ</t>
+  </si>
+  <si>
+    <t>1.8V regulator</t>
+  </si>
+  <si>
+    <t>motor control MOSFET</t>
+  </si>
+  <si>
+    <t>all connectors</t>
   </si>
 </sst>
 </file>
@@ -420,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,6 +599,86 @@
         <v>23</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>